<commit_message>
test POST rates added
</commit_message>
<xml_diff>
--- a/Billing/app/in/rates.xlsx
+++ b/Billing/app/in/rates.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t xml:space="preserve">Product</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Valencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiwi</t>
   </si>
 </sst>
 </file>
@@ -70,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,20 +155,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -309,10 +310,21 @@
         <v>45</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>